<commit_message>
chorus: edited .xlsx file
</commit_message>
<xml_diff>
--- a/sprint1/trabalho_desenvolvido.xlsx
+++ b/sprint1/trabalho_desenvolvido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogonapoles/Developer/2223/SEM4/SCOMP/202223_scomp_2dd_gxx_1211155_1210957/sprint1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae2f95762269e7b3/Área de Trabalho/I.S.E.P/2º ano/2º semestre/202223_scomp_2dd_g04_1211155_1210957/sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB4BF755-8D8E-5241-B039-286DBF8302E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{DB4BF755-8D8E-5241-B039-286DBF8302E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA69E9BB-D95A-4924-9BCE-B257D1029716}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="4220" windowWidth="28040" windowHeight="17440" xr2:uid="{0A9902CA-5268-1542-9599-AEDC1DE4E6A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A9902CA-5268-1542-9599-AEDC1DE4E6A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>José Diogo Nápoles de Sousa Rente</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Ficha Processos</t>
+  </si>
+  <si>
+    <t>Sinais</t>
   </si>
 </sst>
 </file>
@@ -135,6 +138,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -142,9 +148,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,141 +464,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BCD247-5C71-874E-BFAA-FFFAD371E5D8}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
       <c r="D1" s="1">
         <v>1211155</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2">
         <v>1210957</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="B4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="D11" s="3">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="D12" s="3">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>9</v>
       </c>
       <c r="B13" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="D13" s="3">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="D14" s="3">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="D15" s="3">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>1210957</v>
       </c>
+      <c r="D16" s="3">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="3">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1210957</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chorus: update xls file
</commit_message>
<xml_diff>
--- a/sprint1/trabalho_desenvolvido.xlsx
+++ b/sprint1/trabalho_desenvolvido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae2f95762269e7b3/Área de Trabalho/I.S.E.P/2º ano/2º semestre/202223_scomp_2dd_g04_1211155_1210957/sprint1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogonapoles/Developer/2223/SEM4/SCOMP/202223_scomp_2dd_gxx_1211155_1210957/sprint1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{DB4BF755-8D8E-5241-B039-286DBF8302E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA69E9BB-D95A-4924-9BCE-B257D1029716}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDE1A87-D7CC-8C42-932D-14607280219D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0A9902CA-5268-1542-9599-AEDC1DE4E6A1}"/>
+    <workbookView xWindow="7040" yWindow="2100" windowWidth="29040" windowHeight="15720" xr2:uid="{0A9902CA-5268-1542-9599-AEDC1DE4E6A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>José Diogo Nápoles de Sousa Rente</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Sinais</t>
+  </si>
+  <si>
+    <t>Pipes</t>
   </si>
 </sst>
 </file>
@@ -464,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BCD247-5C71-874E-BFAA-FFFAD371E5D8}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -482,7 +485,7 @@
         <v>1211155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -492,7 +495,7 @@
         <v>1210957</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -501,8 +504,12 @@
         <v>3</v>
       </c>
       <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -515,8 +522,14 @@
       <c r="E5" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -529,8 +542,14 @@
       <c r="E6" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -543,8 +562,14 @@
       <c r="E7" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -557,8 +582,14 @@
       <c r="E8" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -571,8 +602,14 @@
       <c r="E9" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -585,8 +622,14 @@
       <c r="E10" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -599,8 +642,14 @@
       <c r="E11" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="3">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -613,8 +662,14 @@
       <c r="E12" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="3">
+        <v>8</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -627,8 +682,14 @@
       <c r="E13" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="3">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -641,8 +702,14 @@
       <c r="E14" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="3">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -655,8 +722,14 @@
       <c r="E15" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="3">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -669,16 +742,28 @@
       <c r="E16" s="2">
         <v>1210957</v>
       </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="3">
+        <v>12</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1210957</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D17" s="3">
         <v>13</v>
       </c>
       <c r="E17" s="1">
         <v>1211155</v>
       </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="3">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1211155</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D18" s="3">
         <v>14</v>
       </c>
@@ -686,7 +771,7 @@
         <v>1210957</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D19" s="3">
         <v>15</v>
       </c>
@@ -694,7 +779,7 @@
         <v>1211155</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D20" s="3">
         <v>16</v>
       </c>
@@ -703,12 +788,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>